<commit_message>
add trade plan for Thursday 20161222
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>LogTime</t>
   </si>
@@ -52,6 +52,21 @@
   </si>
   <si>
     <t xml:space="preserve">NG is very likely to go up lot before Thursday report comes out, which is expected to be -198 to -210, which is already priced. Try to sell all UGAZ on Wednesday at the meanwhile buy back the 477 DGAZ sold at 4.5 </t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>Lessons</t>
+  </si>
+  <si>
+    <t>don't estimate the online trading (after 2:30pm)</t>
+  </si>
+  <si>
+    <t>Good to stick to the trade plan, but sell all UGAZ and bought back DGAZ too early. The trend is obvious (from 8am -930am) but a small dip lure you to act too early. Make 15% a day is good, but you could have made 24%. Need more patience but some being conservative will save your ass in the long run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A great uptrend for NG before the Thursday's report, though the consensus for the report is around -200 but I think this heavily expected report is already priced in during today's trade. Techinically it could reach Monday's gap low at 3.661. Weather is warmer than normal which is not supportive, this could be a bull trap in short term. Hold until 1030 to buy DGAZ when it jump high. One thing to to notice is that, expiration day is coming close, holidays could surpress consumption and today's DGAZ trade volumn is huge, well, UGAZ's trade volum is also huge, something big is going on, be very careful! </t>
   </si>
 </sst>
 </file>
@@ -399,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,10 +425,11 @@
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="139.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="84.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="64.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,26 +445,49 @@
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20161221</v>
+      </c>
+      <c r="B3" s="2">
+        <v>20161221</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>20161221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20161220</v>
       </c>
@@ -464,14 +503,17 @@
       <c r="E5" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>20161213</v>
       </c>
@@ -488,13 +530,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20161212</v>
       </c>
@@ -513,6 +555,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
trading plan for 2016122
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>LogTime</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t xml:space="preserve">A great uptrend for NG before the Thursday's report, though the consensus for the report is around -200 but I think this heavily expected report is already priced in during today's trade. Techinically it could reach Monday's gap low at 3.661. Weather is warmer than normal which is not supportive, this could be a bull trap in short term. Hold until 1030 to buy DGAZ when it jump high. One thing to to notice is that, expiration day is coming close, holidays could surpress consumption and today's DGAZ trade volumn is huge, well, UGAZ's trade volum is also huge, something big is going on, be very careful! </t>
+  </si>
+  <si>
+    <t>Very bad decision buying without knowing the weather could change (turn colder in early Jan) and the fund is not settled. NEVER do it AGAIN! Do not fight the trend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Already under the water and possibly already erased all last week's gain… find a chagne to get out to stop much losses. Two days away from Thursday's report, which could be a small withdraw due to last week's warm weather. If the NG pircce don't pass 3.777, we may have a chance to hold and make profits, becauase that means the turning point of the up-trend </t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -422,30 +428,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="11.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="84.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="64.5546875" customWidth="1"/>
+    <col min="6" max="6" width="64.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -453,103 +460,132 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>20161226</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3">
+        <v>20161227</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>20161221</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B5" s="3">
         <v>20161221</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3">
+      <c r="G5">
         <v>20161221</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>20161220</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B7" s="3">
         <v>20161220</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>20161213</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C9" s="3">
         <v>20161214</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>20161212</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C11" s="3">
         <v>20161213</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
trading plan for 20170103
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>LogTime</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t xml:space="preserve">Already under the water and possibly already erased all last week's gain… find a chagne to get out to stop much losses. Two days away from Thursday's report, which could be a small withdraw due to last week's warm weather. If the NG pircce don't pass 3.777, we may have a chance to hold and make profits, becauase that means the turning point of the up-trend </t>
+  </si>
+  <si>
+    <t>20170103-15min and 20170103-1h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be patient to see -10% in NG today! </t>
+  </si>
+  <si>
+    <t>huge gap down following the new year's long weekend, due to warmer than normal weather forecast in mid Jan. The Ng price may swing up a little more likely for a bull trap in the early morning (like now, around 1030am) and then will resume down trend and continue this to tomorrow, the day before the report day, which is expected to be ~-70, quite bearish but it's probabl6y already priced in by now. The next daily susport area is 3.315 -3.341</t>
   </si>
 </sst>
 </file>
@@ -108,13 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -420,9 +426,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -434,25 +440,26 @@
     <col min="4" max="4" width="12.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="84.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="64.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -460,132 +467,171 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
+        <v>20170103</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>20170103</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>20161226</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C6" s="2">
         <v>20161227</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>20161221</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B8" s="2">
         <v>20161221</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G5">
+      <c r="G8" s="1">
         <v>20161221</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>20161220</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B10" s="2">
         <v>20161220</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>20161213</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C12" s="2">
         <v>20161214</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>20161212</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C14" s="2">
         <v>20161213</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified trade plan for 20170105
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>LogTime</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>huge gap down following the new year's long weekend, due to warmer than normal weather forecast in mid Jan. The Ng price may swing up a little more likely for a bull trap in the early morning (like now, around 1030am) and then will resume down trend and continue this to tomorrow, the day before the report day, which is expected to be ~-70, quite bearish but it's probabl6y already priced in by now. The next daily susport area is 3.315 -3.341</t>
+  </si>
+  <si>
+    <t>hold and watch, don't buy or sell before clear signal</t>
+  </si>
+  <si>
+    <t>Not sure it's a great move to sold most of DGAZ today at 4.31 but it's good and conservative move, as there're always plenty of opportunities out there in the market. As for tomorrow the report day, the consensus is ~-72 to -85, but keep in mind that even the weather is now warmer than normal, the inventory is decreasing than last year and five-year average, so even normal or warmer weather will continue to use up gas in storage, thus this should prevent a total collapse in prices. The current support might be seen around $3.1, and the dropping of NG is slowing down, we can see what will happen around $3.1</t>
   </si>
 </sst>
 </file>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,36 +480,36 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>20170103</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>20170103</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>20170104</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20170105</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2">
+        <v>20170104</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
@@ -513,125 +519,164 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>20161226</v>
+        <v>20170103</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2">
-        <v>20161227</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20170103</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>20161226</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20161227</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>20161221</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B11" s="2">
         <v>20161221</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G11" s="1">
         <v>20161221</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>20161220</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B13" s="2">
         <v>20161220</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>20161213</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C15" s="2">
         <v>20161214</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>20161212</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C17" s="2">
         <v>20161213</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add trade plan for 20170106
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>LogTime</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Not sure it's a great move to sold most of DGAZ today at 4.31 but it's good and conservative move, as there're always plenty of opportunities out there in the market. As for tomorrow the report day, the consensus is ~-72 to -85, but keep in mind that even the weather is now warmer than normal, the inventory is decreasing than last year and five-year average, so even normal or warmer weather will continue to use up gas in storage, thus this should prevent a total collapse in prices. The current support might be seen around $3.1, and the dropping of NG is slowing down, we can see what will happen around $3.1</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>The report came out as -49, way less withdraw than the expected -72~-85. This is very bearish but NG quickly when it touched 3.170 and consolidated around 3.20, where we can feel the support. NG ended up a green candle with very bearish report, which simply means the bearish report were well expected and priced in already. But due to warm weather forecast, the NG continues to see presistence around 3.35, what's interesting is that NG continues to rebound after the outcry 14:30 but quickly drew back after. It's also interesting to notice the volume for DGAZ is relatively small while the volume of UGAZ is larger than normal, I have a strong feeling this could be a profit taking for NG shot and day trade opportunity to buy UGAZ tomorrow (or even hold over the weekend)</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,36 +486,32 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+    <row r="3" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>20170105</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20170106</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>20170104</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2">
-        <v>20170105</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2">
-        <v>20170104</v>
-      </c>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
@@ -519,27 +521,27 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>20170103</v>
+        <v>20170104</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>20170103</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20170105</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="G6" s="2">
+        <v>20170104</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -550,33 +552,35 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>20161226</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2">
-        <v>20161227</v>
-      </c>
-      <c r="D9" s="2" t="s">
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>20170103</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C8" s="1">
+        <v>20170103</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -584,29 +588,29 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>20161221</v>
-      </c>
-      <c r="B11" s="2">
-        <v>20161221</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
+        <v>20161226</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2">
+        <v>20161227</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20161221</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
@@ -614,24 +618,27 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>20161220</v>
+        <v>20161221</v>
       </c>
       <c r="B13" s="2">
-        <v>20161220</v>
+        <v>20161221</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20161221</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -642,19 +649,22 @@
     </row>
     <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>20161213</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>20161220</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20161220</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="2">
-        <v>20161214</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -665,18 +675,41 @@
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
+        <v>20161213</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2">
+        <v>20161214</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>20161212</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C19" s="2">
         <v>20161213</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UGAZ and DGAZ candle graph for 20170105
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>LogTime</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>The report came out as -49, way less withdraw than the expected -72~-85. This is very bearish but NG quickly when it touched 3.170 and consolidated around 3.20, where we can feel the support. NG ended up a green candle with very bearish report, which simply means the bearish report were well expected and priced in already. But due to warm weather forecast, the NG continues to see presistence around 3.35, what's interesting is that NG continues to rebound after the outcry 14:30 but quickly drew back after. It's also interesting to notice the volume for DGAZ is relatively small while the volume of UGAZ is larger than normal, I have a strong feeling this could be a profit taking for NG shot and day trade opportunity to buy UGAZ tomorrow (or even hold over the weekend)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Even though now this is weather-controleld market for NG, but 5 consective selling (with a huge gap down on Sunday opening) will very much lead to a profit taking or huge rebound, especially with a little bit help of weather change. Try to sell DGAZ tomorrow at the first NG dip and get some UGAZ for day-trading or hold until next week </t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,8 +453,8 @@
     <col min="2" max="2" width="11.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="84.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="64.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="95.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="55.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -486,7 +489,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>20170105</v>
       </c>
@@ -502,8 +505,12 @@
       <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2">
+        <v>20170105</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -513,67 +520,67 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>20170104</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C5" s="2">
         <v>20170105</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G5" s="2">
         <v>20170104</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>20170103</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C7" s="1">
         <v>20170103</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
@@ -583,133 +590,125 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+    <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>20161226</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <v>20161227</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>20161226</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>20161221</v>
+      </c>
+      <c r="B12" s="2">
+        <v>20161221</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20161221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>20161220</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20161220</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>20161213</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2">
+        <v>20161214</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>20161212</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>20161227</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C18" s="2">
+        <v>20161213</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>20161221</v>
-      </c>
-      <c r="B13" s="2">
-        <v>20161221</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20161221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>20161220</v>
-      </c>
-      <c r="B15" s="2">
-        <v>20161220</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>20161213</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2">
-        <v>20161214</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>20161212</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2">
-        <v>20161213</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add trade review for 20170106 and NG candle graph
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>LogTime</t>
   </si>
@@ -97,6 +97,23 @@
   </si>
   <si>
     <t xml:space="preserve">Even though now this is weather-controleld market for NG, but 5 consective selling (with a huge gap down on Sunday opening) will very much lead to a profit taking or huge rebound, especially with a little bit help of weather change. Try to sell DGAZ tomorrow at the first NG dip and get some UGAZ for day-trading or hold until next week </t>
+  </si>
+  <si>
+    <t>1. if you found youeself missed today's high and want to sell, wait or sell the previous high, it will come back 
+2. you will have enough time to buy at the bottom, don't guess a low and buy it
+3. A rally failure will lead to bears control 
+4. Down on Monday and Tuesday, with a promising Thursday report, sell on Wednesday or 
+ Thursday when it soars and then buy them back on Friday
+5. A hugh rally (typically on Wed) before a bullish-expected report on Thursday, may
+ lead to profit taking after Thursday's release
+6. You are currently not a good trader, so don't be greedy! 
+7. At the end of May or beginning of June, EIA may adjusted its estimation of gas supply and demand, which lead to the change to storage
+通常有人跟我说，你看我要是牛市赚一点就跑呢？那我就会反问大家，你究竟要赚多点才跑？是否保证永不回来？这些人通常会很沉么，这其实是一个典型的赔钱思维，也是人性的体现。大家炒股的时候往往是牛市，而牛市里任何一次买入都是正确的，任何一次卖出都是错误的，那种说要小赚就走的人，往往会懊悔不已，会在加仓杀回，直到满仓被套。最后是牛市里不断小赚，但熊市里全都回去了。这就是止盈不止损，是最要命，最亏钱的一种做法。而反人性的操作才是正确的，也就是止损不止盈，牛市里持股抱股不放，将盈利放到最大。熊市来了，不管亏损与否坚决离场。
+所以股票越炒战绩越糟糕，并不是您的错，只是市场变化了，而您没有做出适时的调整。所谓居安思危，在得意的时候有几个人会想到学习止损呢？这就是人性，而炒股票，最大的敌人不是市场、不是对手，恰恰是每个人的人性！这就是为何正常思维的人，很难战胜市场的原因。
+最后说句名言，请记住，买入股票的唯一理由，是他未来能够上涨，跟你之前是否亏损赚钱没关系。卖出股票的唯一理由，是他未来要下跌，跟你是否被套也没有任何关系。切记</t>
+  </si>
+  <si>
+    <t>Several fake rallies today looks like a bull trape, trying to lure bulls in. But there's still big pressure around 3.330. NG price is moving slowly within a very narror interval, 3.265~3.330. Weather is still very warm, next Sunday could be gap down again, which will provide a perfect opportunity to bug UGAZ. Pay attention to the volume of DGAZ and UGAZ this a few days, the pattern of UGAZ volume is very similiar to the volumn of DGAZ 5 days ago (starting last Thursday and Friday), which could indicate a low on Monday and then surge!</t>
   </si>
 </sst>
 </file>
@@ -132,13 +149,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,35 +508,29 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>20170105</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2">
         <v>20170106</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="2">
-        <v>20170105</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -520,27 +540,27 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>20170104</v>
+        <v>20170105</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
+        <v>20170106</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2">
         <v>20170105</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="2">
-        <v>20170104</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -551,27 +571,27 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>20170103</v>
+        <v>20170104</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1">
-        <v>20170103</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20170105</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="G7" s="2">
+        <v>20170104</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -582,33 +602,35 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>20161226</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2">
-        <v>20161227</v>
-      </c>
-      <c r="D10" s="2" t="s">
+    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>20170103</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C9" s="1">
+        <v>20170103</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -616,29 +638,29 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>20161221</v>
-      </c>
-      <c r="B12" s="2">
-        <v>20161221</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>20161226</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2">
+        <v>20161227</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20161221</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
@@ -646,24 +668,27 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>20161220</v>
+        <v>20161221</v>
       </c>
       <c r="B14" s="2">
-        <v>20161220</v>
+        <v>20161221</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="G14" s="1">
+        <v>20161221</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -672,21 +697,24 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>20161213</v>
-      </c>
-      <c r="B16" s="2" t="s">
+        <v>20161220</v>
+      </c>
+      <c r="B16" s="2">
+        <v>20161220</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="2">
-        <v>20161214</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -695,20 +723,43 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
+        <v>20161213</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2">
+        <v>20161214</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>20161212</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C20" s="2">
         <v>20161213</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -720,12 +771,540 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:R26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add UGAZ and DGAZ volume and candle graph
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>LogTime</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Several fake rallies today looks like a bull trape, trying to lure bulls in. But there's still big pressure around 3.330. NG price is moving slowly within a very narror interval, 3.265~3.330. Weather is still very warm, next Sunday could be gap down again, which will provide a perfect opportunity to bug UGAZ. Pay attention to the volume of DGAZ and UGAZ this a few days, the pattern of UGAZ volume is very similiar to the volumn of DGAZ 5 days ago (starting last Thursday and Friday), which could indicate a low on Monday and then surge!</t>
+  </si>
+  <si>
+    <t>UGAZ's volume could indicate a big surge/revenge next week</t>
   </si>
 </sst>
 </file>
@@ -469,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,8 +532,12 @@
       <c r="E3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3">
+        <v>20170106</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>

</xml_diff>

<commit_message>
add UGAZ possible buy in price for Monday 20170109
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -116,7 +116,7 @@
     <t>Several fake rallies today looks like a bull trape, trying to lure bulls in. But there's still big pressure around 3.330. NG price is moving slowly within a very narror interval, 3.265~3.330. Weather is still very warm, next Sunday could be gap down again, which will provide a perfect opportunity to bug UGAZ. Pay attention to the volume of DGAZ and UGAZ this a few days, the pattern of UGAZ volume is very similiar to the volumn of DGAZ 5 days ago (starting last Thursday and Friday), which could indicate a low on Monday and then surge!</t>
   </si>
   <si>
-    <t>UGAZ's volume could indicate a big surge/revenge next week</t>
+    <t>UGAZ's volume could indicate a big surge/revenge next week. The previous low 26.79 could be a good buy-in point, or the two previous gap higes at 25.34 and 23.69</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,7 +675,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>20161221</v>
       </c>

</xml_diff>

<commit_message>
add trade plna for Wednesday 20170111
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>LogTime</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t xml:space="preserve">Slightly gap down for like 10 cents at 6pm, but the weather is even warmer after the weekend. There're some suspicous theories that the last report was wrong (because the withdrew was too small) and there will be a correction this coming Thurday. Also, another theory is wandering around about the weather forecast, is about to turn cold soon. People on the forum are saying the temperature is actually lower these days than forecasted. The trading plan for tomorrow might be sell DGAZ and find good point to buy in UGAZ and hold (better in the morning). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NG had a big drop on Monday but met strong support at 3.103, only posted one 1-hour green candle the whole day before 4pm. The weather forecast is still warm (but speculaters are saying Canada's code air will travel south), with the huge UGAZ trading volume, the NG keep rising over the night trading hours, and rised around 6% on Tuesday and totally shadow Monday's red candle. With this trend, the NG prices will very likely to keep going again tomorrow on Wednesday, especially expectin a big withdraw for Thursday's report. Still not sure Tuesday's surge was due to anticipation of weather chagne or more from the profit taking/short recovering angle, but it's probably conservative to sell some UGAZ to lock some profit. Or wait for the price to top, sell and buy back. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be more patient on buying UGAZ while NG price is reducing during the course of day. It is good to get in when having a strong feeling the trend will probably reverse, telling by the UGAZ trading volume, but patience will pay off if wait longer, there will be better enter prices. Normally, a big bottom will give you enough time to enter, because it's big! </t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,13 +536,28 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
+    <row r="3" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>20170110</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>20170111</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5">
+        <v>20170109</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>

</xml_diff>

<commit_message>
update trading plans for Monday 20170130
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -155,10 +155,10 @@
     <t>The uptrend of NG price is quite obvious now, but we can tell the rising of the price is a little bit hesitate. Try to make a few day trades, sell at highs and buy back</t>
   </si>
   <si>
-    <t xml:space="preserve">Due to the weather in 6-10 and 8-14 of NOAA still shows warmer than normal thus gap down to 3.000 at Sunday 6pm opening. I expect this to test 3.270-3.280 tomorrow and plan to buy ugaz around 28.5 to 29, half position. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Glad didn't bought ugaz at 29 last Friday since I may got caught under the water tomorrow. You can afford to miss a few opportunities since the market is always full of opportunities, but you can't affort too many mistakes. Be conservative! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Due to the weather in 6-10 and 8-14 of NOAA still shows warmer than normal thus gap down to 3.000 at Sunday 6pm opening. I expect NG to test 3.270-3.280 tomorrow and plan to buy ugaz around 28.5 to 29, half position. I would buy about half position (only for short terms) when NG comes down to 3.28-3.29, or get clsoer to 3.27 or even dip below 3.27, and if NG continues to go down, wait for 3.17-3.20 to enter full position of UGAZ). Early weekly storage report calls for -60~-70 withdraw by COB last Friday, according to analysts, this is by no means bearch number (or might be priced in during tomorrow's session) , it is said and I quote here "Power demand remains strong, export activity has been robust and production continues to show limited response to the recent upswing in the rig counts. All of these factors will be supportive for natural gas in the future". -Good Luck! </t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20170128</v>
       </c>
@@ -592,10 +592,10 @@
         <v>8</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="G3" s="9">
         <v>20170129</v>
@@ -725,7 +725,7 @@
         <v>20170109</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -733,7 +733,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20170108</v>
       </c>

</xml_diff>

<commit_message>
modify trading plan for Thursday 20170202
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -176,10 +176,10 @@
     <t>Since NG dropped below 3.17 overnight and in the pre-market hours, it is too impatient to buy the rest of UGAZ at 24.99 （ could then lower than 24.50). Patience is very important especially we no longer have the time and stare at the 15min trading all day! We will very likely to get a rebound and then go down back to 3.1 again. It's another opportunity to grasp, be patient and not greedy</t>
   </si>
   <si>
-    <t xml:space="preserve">Weather is still warm for most of US continent, but today's forcast shows a little cold coming in from northeast and great lakes areas. Today small rally were more likely due to short covering, small profit taking by bears since the volume of NG, DGAZ and UGAZ are all relatively quite small. Euro and Asan trades push NG price above 3.22, the previous support, over the night but it was quickly sold back to under 3.170 before US markets opens. Each little rallies that touched 3.170 were sold out and bounced back at 3.15, a very narrow swing interval. Tomorrow's export is expect to be -82, smaller than 5 year average and last week.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Good to sell the 515 UGAZ at 25.75 that was bought at 24.99. For loss of 400 UGAZ bought at 27.55 but sold at 25.9, there should some opportunies to buy back under 25.2 before the report came out. Take it. Hold the rest fund after the report came out. Eventually it would go up anyways, take it and hold over the weekend. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather is still warm for most of US continent, but today's forcast shows a little cold coming in from northeast and great lakes areas. Today small rally were more likely due to short covering, small profit taking by bears since the volume of NG, DGAZ and UGAZ are all relatively quite small. Euro and Asan trades push NG price above 3.22, the previous support, over the night but it was quickly sold back to under 3.170 before US markets opens. Each little rallies that touched 3.170 were sold out and bounced back at 3.15, a very narrow swing interval. Tomorrow's export is expect to be -82, smaller than 5 year average and last week.  The price could seriouly test or even break down 3.10 tomorrow before or after the report, leave half position and prepare for it. </t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +608,7 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
     </row>
-    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20170201</v>
       </c>
@@ -622,10 +622,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>50</v>
       </c>
       <c r="G3" s="12">
         <v>20170202</v>

</xml_diff>

<commit_message>
modify trading plans for 20170222
</commit_message>
<xml_diff>
--- a/NaturalGas/UGAZ and DGAZ.xlsx
+++ b/NaturalGas/UGAZ and DGAZ.xlsx
@@ -206,10 +206,10 @@
     <t>Wednesdy</t>
   </si>
   <si>
-    <t xml:space="preserve">With a bearish outlook for Thirsday's report and a very warm weather to cover most of the courty, and east coast in 8-14 forecast, the NG probably has some more down to go. While some rebounces is expected, but only will provide more selling opportunities. And the only chance to reduce losses is to sell and buy back.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Important lesson: don't hold over the long weekend, especially buy at the last minute of Friday's closing point. Be conservertive and be patient! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">With a bearish outlook for Thirsday's report and a very warm weather to cover most of the courty, and east coast in 8-14 forecast, the NG probably has some more down to go. While some rebounces is expected, but only will provide more selling opportunities. And the only chance to reduce losses is to sell and buy back.  Some expects Thursday's report to show -93, some to expect a -140, not sure which one is correct but last week seems much warmer than the week before. Our only friend right now, is patience and the cold air coming from the west </t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +653,7 @@
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20170221</v>
       </c>
@@ -667,10 +667,10 @@
         <v>58</v>
       </c>
       <c r="E3" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="G3" s="17">
         <v>20170221</v>

</xml_diff>